<commit_message>
Mejoras en descarga de archivos Excel
</commit_message>
<xml_diff>
--- a/App.Web/App_Data/PROCESOS.xlsx
+++ b/App.Web/App_Data/PROCESOS.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\source\repos\GestionProcesosV2\App.Web\App_Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vsilva\source\repos\GestionProcesos\App.Web\App_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{357F0EC3-90A9-47B7-A416-9AC663AF038C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7F8EC09-2F60-4418-8BB8-80F76ACA8A12}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="825" yWindow="-120" windowWidth="23295" windowHeight="13740" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Procesos" sheetId="1" r:id="rId1"/>
     <sheet name="Workflow" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Procesos!$A$1:$H$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Procesos!$A$1:$I$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Workflow!$A$1:$P$1</definedName>
   </definedNames>
   <calcPr calcId="0" iterateDelta="1E-4"/>
@@ -415,7 +415,7 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.7109375" bestFit="1" customWidth="1"/>
@@ -459,7 +459,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H1" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:I1" xr:uid="{8C004D9E-55A6-48F9-B348-7E771A960909}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
@@ -473,7 +473,7 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.7109375" bestFit="1" customWidth="1"/>

</xml_diff>

<commit_message>
Correcciones de reportes, vistas y nuevos filtros
</commit_message>
<xml_diff>
--- a/App.Web/App_Data/PROCESOS.xlsx
+++ b/App.Web/App_Data/PROCESOS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vsilva\source\repos\GestionProcesos\App.Web\App_Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IROCHA\source\repos\GestionProcesos\App.Web\App_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7F8EC09-2F60-4418-8BB8-80F76ACA8A12}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C2C4B8B-3B5C-4512-BB3E-E1D5A42C5519}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Procesos" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="17">
   <si>
     <t>Id</t>
   </si>
@@ -78,6 +78,9 @@
   </si>
   <si>
     <t>Reservado?</t>
+  </si>
+  <si>
+    <t>Id Proceso</t>
   </si>
 </sst>
 </file>
@@ -123,12 +126,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="22" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="22" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -415,9 +418,9 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.85546875" customWidth="1"/>
     <col min="2" max="2" width="19.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.140625" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.140625" style="3" bestFit="1" customWidth="1"/>
@@ -431,7 +434,7 @@
   <sheetData>
     <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -473,7 +476,7 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.7109375" bestFit="1" customWidth="1"/>

</xml_diff>

<commit_message>
Cambios en vistas de cometidos y consulta de los reportes
</commit_message>
<xml_diff>
--- a/App.Web/App_Data/PROCESOS.xlsx
+++ b/App.Web/App_Data/PROCESOS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IROCHA\source\repos\GestionProcesos\App.Web\App_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C2C4B8B-3B5C-4512-BB3E-E1D5A42C5519}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84A6411B-51B9-4C9F-9686-615062C7B701}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Procesos" sheetId="1" r:id="rId1"/>
@@ -30,10 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="17">
-  <si>
-    <t>Id</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="16">
   <si>
     <t>Tipo proceso</t>
   </si>
@@ -56,9 +53,6 @@
     <t>Observación</t>
   </si>
   <si>
-    <t>Workflow id</t>
-  </si>
-  <si>
     <t>Tipo workflow</t>
   </si>
   <si>
@@ -81,6 +75,9 @@
   </si>
   <si>
     <t>Id Proceso</t>
+  </si>
+  <si>
+    <t>Workflow ID</t>
   </si>
 </sst>
 </file>
@@ -414,7 +411,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -434,31 +431,31 @@
   <sheetData>
     <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
       <c r="I1" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -472,75 +469,78 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:P1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="18.42578125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" style="5" customWidth="1"/>
+    <col min="4" max="4" width="20.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.42578125" style="5" customWidth="1"/>
     <col min="6" max="6" width="24.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="31.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="36" customWidth="1"/>
+    <col min="9" max="9" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="37.85546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="70.140625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="49.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12" style="5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20.5703125" style="5" customWidth="1"/>
+    <col min="14" max="14" width="19.28515625" style="5" customWidth="1"/>
+    <col min="15" max="15" width="17.5703125" customWidth="1"/>
     <col min="16" max="16" width="41.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="N1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="P1" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="N1" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>